<commit_message>
Created figure using NY sample
</commit_message>
<xml_diff>
--- a/data/NY data.xlsx
+++ b/data/NY data.xlsx
@@ -1,58 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karinaagadzhanyan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiller/Desktop/Karina/Cam_tidytuesday/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BE47B0D-60E9-E341-9F44-DEA7D546E70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08FA165-D5F6-604B-8545-6219B686A0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="2840" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="distance" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$F$1:$F$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$53</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="116">
-  <si>
-    <t>x</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="111">
   <si>
     <t>Zipcode</t>
   </si>
   <si>
-    <t>DistancefromNYCmi</t>
-  </si>
-  <si>
-    <t>HS</t>
-  </si>
-  <si>
-    <t>SL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NY </t>
-  </si>
-  <si>
     <t xml:space="preserve"> ID</t>
   </si>
   <si>
-    <t>Location Latitude</t>
-  </si>
-  <si>
-    <t>Location Longitude</t>
-  </si>
-  <si>
     <t>R_uvUY8mXa8W5CxO1</t>
   </si>
   <si>
@@ -362,22 +340,28 @@
     <t>12065</t>
   </si>
   <si>
-    <t>Is the Hollywood sign illuminated/lit at night on a typical night?</t>
-  </si>
-  <si>
-    <t>Is she holding the torch in her left or right hand?</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>holly_sign_acc</t>
+  </si>
+  <si>
+    <t>statof_lib_acc</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>long</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="12"/>
@@ -862,8 +846,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1220,485 +1204,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>11763</v>
-      </c>
-      <c r="C2">
-        <v>53.12</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>11783</v>
-      </c>
-      <c r="C3">
-        <v>53.12</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>12065</v>
-      </c>
-      <c r="C4">
-        <v>149.13999999999999</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>12192</v>
-      </c>
-      <c r="C5">
-        <v>114.17</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>12308</v>
-      </c>
-      <c r="C6">
-        <v>145.13</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>12309</v>
-      </c>
-      <c r="C7">
-        <v>145.13</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>12603</v>
-      </c>
-      <c r="C8">
-        <v>68.28</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>12790</v>
-      </c>
-      <c r="C9">
-        <v>64.64</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>12803</v>
-      </c>
-      <c r="C10">
-        <v>179.63</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>13036</v>
-      </c>
-      <c r="C11">
-        <v>208.95</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>13045</v>
-      </c>
-      <c r="C12">
-        <v>172.03</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>13063</v>
-      </c>
-      <c r="C13">
-        <v>179.7</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>13203</v>
-      </c>
-      <c r="C14">
-        <v>195.27</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>13204</v>
-      </c>
-      <c r="C15">
-        <v>195.27</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>13205</v>
-      </c>
-      <c r="C16">
-        <v>195.27</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>13355</v>
-      </c>
-      <c r="C17">
-        <v>163.59</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18">
-        <v>13417</v>
-      </c>
-      <c r="C18">
-        <v>177.94</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19">
-        <v>13619</v>
-      </c>
-      <c r="C19">
-        <v>239.91</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20">
-        <v>13760</v>
-      </c>
-      <c r="C20">
-        <v>142.68</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21">
-        <v>14150</v>
-      </c>
-      <c r="C21">
-        <v>297.06</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <v>14225</v>
-      </c>
-      <c r="C22">
-        <v>292.33999999999997</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>14420</v>
-      </c>
-      <c r="C23">
-        <v>265.75</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24">
-        <v>14510</v>
-      </c>
-      <c r="C24">
-        <v>243.08</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25">
-        <v>14621</v>
-      </c>
-      <c r="C25">
-        <v>250.66</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26">
-        <v>14624</v>
-      </c>
-      <c r="C26">
-        <v>250.66</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27">
-        <v>14904</v>
-      </c>
-      <c r="C27">
-        <v>172.74</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1709,27 +1219,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>42.7956</v>
@@ -1738,18 +1248,18 @@
         <v>-77.804599999999994</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>43.321100000000001</v>
@@ -1758,18 +1268,18 @@
         <v>-76.403400000000005</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>40.6372</v>
@@ -1778,18 +1288,18 @@
         <v>-73.903700000000001</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>43.0745</v>
@@ -1798,18 +1308,18 @@
         <v>-76.146600000000007</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>43.023099999999999</v>
@@ -1818,18 +1328,18 @@
         <v>-75.264899999999997</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>40.761600000000001</v>
@@ -1838,18 +1348,18 @@
         <v>-72.850800000000007</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>40.68</v>
@@ -1858,18 +1368,18 @@
         <v>-73.775000000000006</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="34">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>40.725200000000001</v>
@@ -1878,18 +1388,18 @@
         <v>-73.944000000000003</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>40.8703</v>
@@ -1898,18 +1408,18 @@
         <v>-73.852500000000006</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="34">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>41.927199999999999</v>
@@ -1918,18 +1428,18 @@
         <v>-73.888800000000003</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="34">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>43.258499999999998</v>
@@ -1938,18 +1448,18 @@
         <v>-77.669499999999999</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>43.214300000000001</v>
@@ -1958,18 +1468,18 @@
         <v>-77.9392</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>40.918599999999998</v>
@@ -1978,18 +1488,18 @@
         <v>-73.893199999999993</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="34">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>40.765300000000003</v>
@@ -1998,18 +1508,18 @@
         <v>-73.9589</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="34">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>43.033299999999997</v>
@@ -2018,18 +1528,18 @@
         <v>-74.981200000000001</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="34">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>41.134099999999997</v>
@@ -2038,18 +1548,18 @@
         <v>-73.783100000000005</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1">
         <v>28.1951</v>
@@ -2058,18 +1568,18 @@
         <v>-81.606200000000001</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1">
         <v>42.976700000000001</v>
@@ -2078,18 +1588,18 @@
         <v>-78.795900000000003</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="34">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
         <v>40.680500000000002</v>
@@ -2098,18 +1608,18 @@
         <v>-73.844200000000001</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="34">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>40.770600000000002</v>
@@ -2118,18 +1628,18 @@
         <v>-73.928299999999993</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
         <v>40.703499999999998</v>
@@ -2138,18 +1648,18 @@
         <v>-73.923500000000004</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="34">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
         <v>42.976700000000001</v>
@@ -2158,18 +1668,18 @@
         <v>-78.795900000000003</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="34">
       <c r="A24" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
         <v>40.713000000000001</v>
@@ -2178,18 +1688,18 @@
         <v>-73.559700000000007</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="34">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
         <v>42.4754</v>
@@ -2198,18 +1708,18 @@
         <v>-73.822000000000003</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="34">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1">
         <v>40.822000000000003</v>
@@ -2218,18 +1728,18 @@
         <v>-73.86</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="34">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
         <v>43.084200000000003</v>
@@ -2238,18 +1748,18 @@
         <v>-75.228700000000003</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="34">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
         <v>40.877699999999997</v>
@@ -2258,18 +1768,18 @@
         <v>-73.908000000000001</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="34">
       <c r="A29" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
         <v>40.872999999999998</v>
@@ -2278,18 +1788,18 @@
         <v>-73.823300000000003</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="34">
       <c r="A30" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
         <v>42.722999999999999</v>
@@ -2298,18 +1808,18 @@
         <v>-73.817700000000002</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="34">
       <c r="A31" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1">
         <v>41.691899999999997</v>
@@ -2318,18 +1828,18 @@
         <v>-73.864199999999997</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="34">
       <c r="A32" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1">
         <v>40.735900000000001</v>
@@ -2338,18 +1848,18 @@
         <v>-73.990399999999994</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="34">
       <c r="A33" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1">
         <v>43.018799999999999</v>
@@ -2358,18 +1868,18 @@
         <v>-76.165000000000006</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="34">
       <c r="A34" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1">
         <v>40.725200000000001</v>
@@ -2378,18 +1888,18 @@
         <v>-73.944000000000003</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="34">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1">
         <v>40.780900000000003</v>
@@ -2398,18 +1908,18 @@
         <v>-73.950199999999995</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="34">
       <c r="A36" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1">
         <v>42.848199999999999</v>
@@ -2418,18 +1928,18 @@
         <v>-73.786299999999997</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="34">
       <c r="A37" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1">
         <v>40.738</v>
@@ -2438,18 +1948,18 @@
         <v>-73.985799999999998</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="34">
       <c r="A38" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1">
         <v>41.721800000000002</v>
@@ -2458,18 +1968,18 @@
         <v>-74.414100000000005</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="34">
       <c r="A39" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1">
         <v>45.503300000000003</v>
@@ -2478,18 +1988,18 @@
         <v>-122.7744</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="34">
       <c r="A40" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1">
         <v>40.662700000000001</v>
@@ -2498,18 +2008,18 @@
         <v>-73.913799999999995</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="34">
       <c r="A41" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1">
         <v>40.725200000000001</v>
@@ -2518,18 +2028,18 @@
         <v>-73.944000000000003</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="34">
       <c r="A42" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1">
         <v>42.0852</v>
@@ -2538,18 +2048,18 @@
         <v>-76.842200000000005</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="34">
       <c r="A43" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1">
         <v>40.6462</v>
@@ -2558,18 +2068,18 @@
         <v>-73.9559</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="34">
       <c r="A44" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1">
         <v>40.673699999999997</v>
@@ -2578,18 +2088,18 @@
         <v>-73.533600000000007</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="34">
       <c r="A45" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1">
         <v>43.323799999999999</v>
@@ -2598,18 +2108,18 @@
         <v>-73.677199999999999</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="34">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1">
         <v>40.680500000000002</v>
@@ -2618,18 +2128,18 @@
         <v>-73.844200000000001</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="34">
       <c r="A47" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1">
         <v>40.750300000000003</v>
@@ -2638,18 +2148,18 @@
         <v>-74.001400000000004</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="34">
       <c r="A48" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1">
         <v>40.706400000000002</v>
@@ -2658,18 +2168,18 @@
         <v>-73.947299999999998</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="34">
       <c r="A49" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1">
         <v>40.703499999999998</v>
@@ -2678,18 +2188,18 @@
         <v>-73.923500000000004</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="34">
       <c r="A50" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1">
         <v>40.824100000000001</v>
@@ -2698,18 +2208,18 @@
         <v>-73.8977</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="34">
       <c r="A51" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B51" s="1">
         <v>40.582799999999999</v>
@@ -2718,18 +2228,18 @@
         <v>-73.953199999999995</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="34">
       <c r="A52" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1">
         <v>43.018799999999999</v>
@@ -2738,18 +2248,18 @@
         <v>-76.165000000000006</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="34">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1">
         <v>42.848199999999999</v>
@@ -2758,13 +2268,13 @@
         <v>-73.786299999999997</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>